<commit_message>
cambios decimales en ICX y NPS
</commit_message>
<xml_diff>
--- a/Resultado/informe_mensual_febrero_2025.xlsx
+++ b/Resultado/informe_mensual_febrero_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slenis.BANCOLOMBIA\Documents\projecto_dashboard\Resultado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD6CBC6-9EB9-4A13-ACEC-6EB3512C2854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25BAC6F1-FCE8-4F6C-AEE8-BFF0CC7F7C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -116,12 +116,6 @@
     <t>10.5%</t>
   </si>
   <si>
-    <t>4.8</t>
-  </si>
-  <si>
-    <t>81.32%</t>
-  </si>
-  <si>
     <t>1.17%</t>
   </si>
   <si>
@@ -165,6 +159,12 @@
   </si>
   <si>
     <t>14,029,663,120,677</t>
+  </si>
+  <si>
+    <t>81.16%</t>
+  </si>
+  <si>
+    <t>4.80</t>
   </si>
 </sst>
 </file>
@@ -223,11 +223,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,7 +537,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,10 +679,10 @@
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -691,10 +693,10 @@
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -705,10 +707,10 @@
         <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -747,10 +749,10 @@
         <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -761,38 +763,38 @@
         <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="B17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" t="s">
-        <v>27</v>
+      <c r="B17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
-      <c r="B18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" t="s">
-        <v>28</v>
+      <c r="B18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -811,7 +813,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B20">
         <v>19411918</v>
@@ -825,16 +827,16 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" t="s">
         <v>40</v>
       </c>
-      <c r="B21" t="s">
+      <c r="D21" t="s">
         <v>41</v>
-      </c>
-      <c r="C21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>